<commit_message>
Konzept 2 und balltransport
</commit_message>
<xml_diff>
--- a/bin/Berechnungen.xlsx
+++ b/bin/Berechnungen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mindistwinkel" sheetId="1" r:id="rId1"/>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q146"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8466,8 +8466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8952,7 +8952,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Berechnungen erfüllt und Budget
</commit_message>
<xml_diff>
--- a/bin/Berechnungen.xlsx
+++ b/bin/Berechnungen.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Mindistwinkel" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="3" r:id="rId2"/>
     <sheet name="Foglio1" sheetId="2" r:id="rId3"/>
     <sheet name="Foglio3" sheetId="4" r:id="rId4"/>
+    <sheet name="Foglio4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
   <si>
     <t>m</t>
   </si>
@@ -174,14 +175,52 @@
   <si>
     <t>a (rad)</t>
   </si>
+  <si>
+    <t>I Ball</t>
+  </si>
+  <si>
+    <t>I Ball gesamt</t>
+  </si>
+  <si>
+    <t>I Rad</t>
+  </si>
+  <si>
+    <t>m rad</t>
+  </si>
+  <si>
+    <t>I Gesamt</t>
+  </si>
+  <si>
+    <t>kg*m^2</t>
+  </si>
+  <si>
+    <t>Nm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abstand </t>
+  </si>
+  <si>
+    <t>Drehzahl mit eine Wurfhöhe von 0.4m, ein Abwurfwinkel von 45°,
+ein Rad mit Radius r = 0,05m und abstand x</t>
+  </si>
+  <si>
+    <t>Geschwindigkeit m/s</t>
+  </si>
+  <si>
+    <t>Drezahl U/min</t>
+  </si>
+  <si>
+    <t>Winkel °</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -212,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -337,11 +376,185 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -375,6 +588,48 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -770,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q146"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2274,7 +2529,7 @@
         <v>1.85</v>
       </c>
       <c r="K30" s="23">
-        <f t="shared" si="9"/>
+        <f>(SQRT(C30)*I30)/(SQRT(2)*SQRT(I30*H30+A30-B30)*F30)</f>
         <v>4.1433681950799395</v>
       </c>
       <c r="L30" s="23">
@@ -8467,7 +8722,7 @@
   <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8949,20 +9204,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -8973,7 +9231,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -8984,7 +9242,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <f>0.075*5</f>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -8996,7 +9260,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -9008,7 +9272,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -9017,10 +9281,339 @@
         <v>954.92965855137197</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>4.9000000000000005E-5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
       <c r="F11" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13">
+        <f>B11+0.06*B4*B4</f>
+        <v>1.9900000000000001E-4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16">
+        <v>0.3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17">
+        <f>0.5*B16*B4*B4</f>
+        <v>3.7500000000000001E-4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
+        <f>B17+B13</f>
+        <v>5.7400000000000007E-4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <f>((B3/B4)^2)/(2*PI())</f>
+        <v>1591.5494309189535</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <f>B22*B20</f>
+        <v>0.91354937334747943</v>
+      </c>
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="45">
+        <v>1.75</v>
+      </c>
+      <c r="B5" s="46">
+        <f>(SQRT(9.81)*A5)/(SQRT(2)*SQRT(A5*TAN(((45/180)*PI())))*COS(((45/180)*PI())))</f>
+        <v>4.1433681950799404</v>
+      </c>
+      <c r="C5" s="50">
+        <f>((B5/0.05)/(2*PI()))*60</f>
+        <v>791.32503515606038</v>
+      </c>
+      <c r="D5" s="54">
+        <f>ACOS(1.75/A5)*(180/PI())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="42">
+        <v>1.76</v>
+      </c>
+      <c r="B6" s="40">
+        <f t="shared" ref="B6:B15" si="0">(SQRT(9.81)*A6)/(SQRT(2)*SQRT(A6*TAN(((45/180)*PI())))*COS(((45/180)*PI())))</f>
+        <v>4.1551895263633876</v>
+      </c>
+      <c r="C6" s="41">
+        <f t="shared" ref="C6:C15" si="1">((B6/0.05)/(2*PI()))*60</f>
+        <v>793.58274312528545</v>
+      </c>
+      <c r="D6" s="52">
+        <f t="shared" ref="D6:D15" si="2">ACOS(1.75/A6)*(180/PI())</f>
+        <v>6.1106462488773463</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="42">
+        <v>1.77</v>
+      </c>
+      <c r="B7" s="40">
+        <f t="shared" si="0"/>
+        <v>4.1669773217525439</v>
+      </c>
+      <c r="C7" s="41">
+        <f t="shared" si="1"/>
+        <v>795.83404621049351</v>
+      </c>
+      <c r="D7" s="52">
+        <f t="shared" si="2"/>
+        <v>8.6213600928398897</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="42">
+        <v>1.78</v>
+      </c>
+      <c r="B8" s="40">
+        <f t="shared" si="0"/>
+        <v>4.1787318650518843</v>
+      </c>
+      <c r="C8" s="41">
+        <f t="shared" si="1"/>
+        <v>798.0789986143468</v>
+      </c>
+      <c r="D8" s="52">
+        <f t="shared" si="2"/>
+        <v>10.534164940871936</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="42">
+        <v>1.79</v>
+      </c>
+      <c r="B9" s="40">
+        <f t="shared" si="0"/>
+        <v>4.1904534360854075</v>
+      </c>
+      <c r="C9" s="41">
+        <f t="shared" si="1"/>
+        <v>800.31765377929241</v>
+      </c>
+      <c r="D9" s="52">
+        <f t="shared" si="2"/>
+        <v>12.135374584375702</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="42">
+        <v>1.8</v>
+      </c>
+      <c r="B10" s="40">
+        <f t="shared" si="0"/>
+        <v>4.2021423107743496</v>
+      </c>
+      <c r="C10" s="41">
+        <f t="shared" si="1"/>
+        <v>802.55006440240459</v>
+      </c>
+      <c r="D10" s="52">
+        <f t="shared" si="2"/>
+        <v>13.536202737381151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="42">
+        <v>1.81</v>
+      </c>
+      <c r="B11" s="40">
+        <f t="shared" si="0"/>
+        <v>4.213798761212975</v>
+      </c>
+      <c r="C11" s="41">
+        <f t="shared" si="1"/>
+        <v>804.7762824498601</v>
+      </c>
+      <c r="D11" s="52">
+        <f t="shared" si="2"/>
+        <v>14.793844003936069</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="42">
+        <v>1.82</v>
+      </c>
+      <c r="B12" s="40">
+        <f t="shared" si="0"/>
+        <v>4.2254230557424659</v>
+      </c>
+      <c r="C12" s="41">
+        <f t="shared" si="1"/>
+        <v>806.99635917104956</v>
+      </c>
+      <c r="D12" s="52">
+        <f t="shared" si="2"/>
+        <v>15.942368605628653</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="42">
+        <v>1.83</v>
+      </c>
+      <c r="B13" s="40">
+        <f t="shared" si="0"/>
+        <v>4.2370154590230147</v>
+      </c>
+      <c r="C13" s="41">
+        <f t="shared" si="1"/>
+        <v>809.21034511234643</v>
+      </c>
+      <c r="D13" s="52">
+        <f t="shared" si="2"/>
+        <v>17.004037075011659</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="42">
+        <v>1.84</v>
+      </c>
+      <c r="B14" s="40">
+        <f t="shared" si="0"/>
+        <v>4.2485762321041145</v>
+      </c>
+      <c r="C14" s="41">
+        <f t="shared" si="1"/>
+        <v>811.41829013053132</v>
+      </c>
+      <c r="D14" s="52">
+        <f t="shared" si="2"/>
+        <v>17.99435512930879</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="43">
+        <v>1.85</v>
+      </c>
+      <c r="B15" s="44">
+        <f t="shared" si="0"/>
+        <v>4.2601056324931665</v>
+      </c>
+      <c r="C15" s="49">
+        <f t="shared" si="1"/>
+        <v>813.62024340589517</v>
+      </c>
+      <c r="D15" s="53">
+        <f t="shared" si="2"/>
+        <v>18.92464441605123</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
WIchtige Berechnungen und Kosten
</commit_message>
<xml_diff>
--- a/bin/Berechnungen.xlsx
+++ b/bin/Berechnungen.xlsx
@@ -1025,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q146"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2584,7 +2584,7 @@
         <v>1.85</v>
       </c>
       <c r="K31" s="16">
-        <f t="shared" si="9"/>
+        <f>(SQRT(C31)*I31)/(SQRT(2)*SQRT(I31*H31+A31-B31)*F31)</f>
         <v>4.175204948208953</v>
       </c>
       <c r="L31" s="16">
@@ -8722,7 +8722,7 @@
   <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="N9" sqref="N8:N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9207,12 +9207,13 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -9374,7 +9375,7 @@
   <dimension ref="B1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>